<commit_message>
Made city markers transparent (what a lot of work!)
</commit_message>
<xml_diff>
--- a/cities-test.xlsx
+++ b/cities-test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>name</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>Charleston</t>
+  </si>
+  <si>
+    <t>col</t>
   </si>
 </sst>
 </file>
@@ -383,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -394,7 +397,7 @@
     <col min="1" max="1" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -404,8 +407,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -415,8 +421,11 @@
       <c r="C2">
         <v>-77.410499999999999</v>
       </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -426,8 +435,11 @@
       <c r="C3">
         <v>-77.201599999999999</v>
       </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -436,6 +448,9 @@
       </c>
       <c r="C4">
         <v>-81.632599999999996</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed the cities a bit.
</commit_message>
<xml_diff>
--- a/cities-test.xlsx
+++ b/cities-test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>name</t>
   </si>
@@ -28,13 +28,16 @@
     <t>Frederick</t>
   </si>
   <si>
-    <t>Gathersburg</t>
-  </si>
-  <si>
     <t>Charleston</t>
   </si>
   <si>
-    <t>col</t>
+    <t>Morgantown</t>
+  </si>
+  <si>
+    <t>Bowie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
   </si>
 </sst>
 </file>
@@ -386,10 +389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -397,7 +400,7 @@
     <col min="1" max="1" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -407,11 +410,9 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -421,36 +422,41 @@
       <c r="C2">
         <v>-77.410499999999999</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3">
-        <v>39.143999999999998</v>
+        <v>38.349800000000002</v>
       </c>
       <c r="C3">
-        <v>-77.201599999999999</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
+        <v>-81.632599999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4">
-        <v>38.349800000000002</v>
+        <v>39.6295</v>
       </c>
       <c r="C4">
-        <v>-81.632599999999996</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
+        <v>-79.9559</v>
+      </c>
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>39.006799999999998</v>
+      </c>
+      <c r="C5">
+        <v>-76.7791</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made cities transparent, added Baltimore, changed up counties slightly.
</commit_message>
<xml_diff>
--- a/cities-test.xlsx
+++ b/cities-test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>name</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t xml:space="preserve">   </t>
+  </si>
+  <si>
+    <t>Baltimore</t>
   </si>
 </sst>
 </file>
@@ -389,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,6 +462,17 @@
         <v>-76.7791</v>
       </c>
     </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>39.290399999999998</v>
+      </c>
+      <c r="C6">
+        <v>-76.612200000000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>

</xml_diff>